<commit_message>
#docs #feature gitbook und tweets class & streamlit
</commit_message>
<xml_diff>
--- a/exported_DataFrame.xlsx
+++ b/exported_DataFrame.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Tweet</t>
   </si>
@@ -22,6 +22,9 @@
     <t>Timestamp of Tweet</t>
   </si>
   <si>
+    <t>Retweets</t>
+  </si>
+  <si>
     <t>Following</t>
   </si>
   <si>
@@ -31,89 +34,72 @@
     <t>User created</t>
   </si>
   <si>
-    <t>Binance - BTC Market
-#SC - Unusual buying activity
-4.71 BTC in 5 minutes (12%)
-P: 0.00000029 ❇ (3.57%)
-24H Vol: 41.08 BTC</t>
-  </si>
-  <si>
-    <t>DYDX
- Falling trend break and retest + cup handle retest = 99% success, the journey to the goal begins ⏳🔥 #bnb… https://t.co/uPwCJNno1r</t>
-  </si>
-  <si>
-    <t>NFT membership, NFT membership, NFT membership! 🙌🙌
-Did someone say NFT membership? 👀
-Get ready for it! 🔥🔥… https://t.co/nwtnEnNAfE</t>
-  </si>
-  <si>
-    <t>RT @EHAA80: @WorkQuest_co is a global end-to-end #jobs #marketplace powered by #DeFi aiming to bring #Blockchain to the #Labor Market.
-#Ma…</t>
-  </si>
-  <si>
-    <t>RT @PiratesWorldNFT: 🤑 1,500 $BUSD GIVEAWAY 🤑
-🎉 Follow us.
-💪🏼 Retweet this post.
-🤩 Tag 2️⃣ Friends.
-❗️Winner announced in 7️⃣ days.
-☠️…</t>
-  </si>
-  <si>
-    <t>@SpaceX @elonmusk #btc     /#mtn money makes us rich #medical_chain makes us millionaires🚀🚀🚀🚀🚀🐳🐳🐳🐳🐳🐳🐳🐳#Huobiglobal</t>
-  </si>
-  <si>
-    <t>RT @papa_woody21: Just got this tattoo so that my wife will think I’m listening when I’m really Tweeting and checking my #crypto @2billiond…</t>
-  </si>
-  <si>
-    <t>RT @ThxuToken: #Airdrop Campaign
-Winners: 2,000 Winners × 5,000 $ThxU
-Period: April 1st~15th
-[Step]
-•Visit Airdrop page
-•Follow &amp;amp; RT on Twi…</t>
-  </si>
-  <si>
-    <t>Signal 1624177 01-Apr 13:44 UTC
-HEART/BTC at KUCOIN
-Buy: 0.00000091 - 0.00000097
-Ask: 0.00000096
-Target 1: 0.0000… https://t.co/R2SRdAHmjl</t>
-  </si>
-  <si>
-    <t>@WatcherGuru By now I’d should became clear to everybody that in time nobody will be willing to sell their ETH or B… https://t.co/FIc0ATNuTI</t>
-  </si>
-  <si>
-    <t>01-04-2022 13:44</t>
-  </si>
-  <si>
-    <t>29-04-2019 20:48</t>
-  </si>
-  <si>
-    <t>01-04-2022 10:54</t>
-  </si>
-  <si>
-    <t>16-02-2022 21:42</t>
-  </si>
-  <si>
-    <t>16-10-2021 13:43</t>
-  </si>
-  <si>
-    <t>24-08-2011 08:43</t>
-  </si>
-  <si>
-    <t>03-10-2021 13:32</t>
-  </si>
-  <si>
-    <t>08-05-2021 06:29</t>
-  </si>
-  <si>
-    <t>18-11-2021 14:59</t>
-  </si>
-  <si>
-    <t>01-05-2020 15:36</t>
-  </si>
-  <si>
-    <t>07-10-2011 06:32</t>
+    <t>{'full_text': '🩸 TheCult - Official 🩸\nPRIVATE SALE NOW OPEN \nBSCs only Official $CULT\n\n🩸 Join us 🩸\n❗️10% REWARDS ❗️\n❗️CHARITY ❗️\n❗️NFTs and NFT Staking ❗️\n❗️P2E ❗️\n‼️Plus much more ‼️\n\nJOIN THE FAMILY-\n🩸 https://t.co/PYIDfPPz8Y 🩸\n#nft #P2E #Crypto #CoinMarketCap #CoinGecko #BNB #BTC https://t.co/mLlx2hDjKI', 'display_text_range': [0, 268], 'entities': {'hashtags': [{'text': 'nft', 'indices': [215, 219]}, {'text': 'P2E', 'indices': [220, 224]}, {'text': 'Crypto', 'indices': [225, 232]}, {'text': 'CoinMarketCap', 'indices': [233, 247]}, {'text': 'CoinGecko', 'indices': [248, 258]}, {'text': 'BNB', 'indices': [259, 263]}, {'text': 'BTC', 'indices': [264, 268]}], 'urls': [{'url': 'https://t.co/PYIDfPPz8Y', 'expanded_url': 'https://t.me/TheCultOfficial', 'display_url': 't.me/TheCultOfficial', 'indices': [189, 212]}], 'user_mentions': [], 'symbols': [{'text': 'CULT', 'indices': [65, 70]}], 'media': [{'id': 1511276368897662976, 'id_str': '1511276368897662976', 'indices': [269, 292], 'media_url': 'http://pbs.twimg.com/media/FPkh2bWWYAAGzM9.jpg', 'media_url_https': 'https://pbs.twimg.com/media/FPkh2bWWYAAGzM9.jpg', 'url': 'https://t.co/mLlx2hDjKI', 'display_url': 'pic.twitter.com/mLlx2hDjKI', 'expanded_url': 'https://twitter.com/OfficialTheCult/status/1511276372697788421/photo/1', 'type': 'photo', 'sizes': {'small': {'w': 680, 'h': 453, 'resize': 'fit'}, 'thumb': {'w': 150, 'h': 150, 'resize': 'crop'}, 'large': {'w': 800, 'h': 533, 'resize': 'fit'}, 'medium': {'w': 800, 'h': 533, 'resize': 'fit'}}}]}, 'extended_entities': {'media': [{'id': 1511276368897662976, 'id_str': '1511276368897662976', 'indices': [269, 292], 'media_url': 'http://pbs.twimg.com/media/FPkh2bWWYAAGzM9.jpg', 'media_url_https': 'https://pbs.twimg.com/media/FPkh2bWWYAAGzM9.jpg', 'url': 'https://t.co/mLlx2hDjKI', 'display_url': 'pic.twitter.com/mLlx2hDjKI', 'expanded_url': 'https://twitter.com/OfficialTheCult/status/1511276372697788421/photo/1', 'type': 'photo', 'sizes': {'small': {'w': 680, 'h': 453, 'resize': 'fit'}, 'thumb': {'w': 150, 'h': 150, 'resize': 'crop'}, 'large': {'w': 800, 'h': 533, 'resize': 'fit'}, 'medium': {'w': 800, 'h': 533, 'resize': 'fit'}}}]}}</t>
+  </si>
+  <si>
+    <t>Promote it on @nftswind</t>
+  </si>
+  <si>
+    <t>RT @_Adammayer: ⚠️2013 - You missed #BTC
+⚠️ 2014 - You missed #DOGE
+⚠️ 2015 - You missed #XRP
+⚠️ 2016 - You missed #ETH
+⚠️ 2017 - You misse…</t>
+  </si>
+  <si>
+    <t>{'full_text': '@syndicate__eth @nftwhalealert 🚨Highest paying BSC Node Project \n💰CRAO Token \n💎Diamond Hands\n💵Nodes Income\n🌶Rewards every 20 minutes\n🚀Launchpad, Escrow Service, Trading Bot in active development\n🐳BUY HERE: https://t.co/qsX00GH6vZ\n\n#CRAOTOKEN  #gems #lowcap #BSCGem #memecoin #BSC #ETH #BTC #SAFEMOON', 'display_text_range': [31, 299], 'entities': {'hashtags': [{'text': 'CRAOTOKEN', 'indices': [231, 241]}, {'text': 'gems', 'indices': [243, 248]}, {'text': 'lowcap', 'indices': [249, 256]}, {'text': 'BSCGem', 'indices': [257, 264]}, {'text': 'memecoin', 'indices': [265, 274]}, {'text': 'BSC', 'indices': [275, 279]}, {'text': 'ETH', 'indices': [280, 284]}, {'text': 'BTC', 'indices': [285, 289]}, {'text': 'SAFEMOON', 'indices': [290, 299]}], 'urls': [{'url': 'https://t.co/qsX00GH6vZ', 'expanded_url': 'https://craotoken.com/swap?from=bnb&amp;ref=0xD0956C29c2b5F7012e9Eb4336D67ee0aBde4e906', 'display_url': 'craotoken.com/swap?from=bnb&amp;…', 'indices': [206, 229]}], 'user_mentions': [{'screen_name': 'syndicate__eth', 'name': 'syndicate eth', 'id': 1482449610807275522, 'id_str': '1482449610807275522', 'indices': [0, 15]}, {'screen_name': 'nftwhalealert', 'name': 'NFT Whale Alert', 'id': 1424994036293586947, 'id_str': '1424994036293586947', 'indices': [16, 30]}], 'symbols': []}}</t>
+  </si>
+  <si>
+    <t>Biggest future BTC whale explains why Bitcoin was chosen for ‘decentralized Forex reserve’ https://t.co/5e4HNEzXil</t>
+  </si>
+  <si>
+    <t>{'full_text': '@ZoroToken 🚀YEAR OF THE $RATS🐭\n@ratscoinx1000\n\n and join our ARMY!\n\nBSC Contract 0x57b798d2252557f13a9148a075a72816f2707356\n\nTG: https://t.co/rI3HQJHl08\n\n#ElonMusk #RATSCOIN #BNB\xa0\xa0  #BNBChain #BSC #BTC\xa0\xa0#memecoin #NFT #100xGems #ATH #BSCGems #SHIB #altcoins #BEP20 #CoinMarketCap #HUHOBI', 'display_text_range': [11, 287], 'entities': {'hashtags': [{'text': 'ElonMusk', 'indices': [154, 163]}, {'text': 'RATSCOIN', 'indices': [164, 173]}, {'text': 'BNB', 'indices': [174, 178]}, {'text': 'BNBChain', 'indices': [182, 191]}, {'text': 'BSC', 'indices': [192, 196]}, {'text': 'BTC', 'indices': [197, 201]}, {'text': 'memecoin', 'indices': [203, 212]}, {'text': 'NFT', 'indices': [213, 217]}, {'text': '100xGems', 'indices': [218, 227]}, {'text': 'ATH', 'indices': [228, 232]}, {'text': 'BSCGems', 'indices': [233, 241]}, {'text': 'SHIB', 'indices': [242, 247]}, {'text': 'altcoins', 'indices': [248, 257]}, {'text': 'BEP20', 'indices': [258, 264]}, {'text': 'CoinMarketCap', 'indices': [265, 279]}, {'text': 'HUHOBI', 'indices': [280, 287]}], 'urls': [{'url': 'https://t.co/rI3HQJHl08', 'expanded_url': 'http://t.me/ratscoinx1000', 'display_url': 't.me/ratscoinx1000', 'indices': [129, 152]}], 'user_mentions': [{'screen_name': 'ZoroToken', 'name': 'Zoro Inu Official', 'id': 2419116015, 'id_str': '2419116015', 'indices': [0, 10]}, {'screen_name': 'ratscoinx1000', 'name': 'RatsCoin', 'id': 193415220, 'id_str': '193415220', 'indices': [31, 45]}], 'symbols': []}}</t>
+  </si>
+  <si>
+    <t>RT @BitninjaX: The Luna Foundation Guard are in #Bitcoin accumulation mode throughout 2022, adding a total of 30,727 #BTC to their balance…</t>
+  </si>
+  <si>
+    <t>$BTC Guys, Don't miss the next move in a few hours...
+https://t.co/i6wbHlrvn7</t>
+  </si>
+  <si>
+    <t>{'full_text': '@skulls_humanity @cryptoBILLnfts 🚨Highest paying BSC Node Project \n💰CRAO Token \n💎Diamond Hands\n💵Nodes Income\n🌶Rewards every 20 minutes\n🚀Launchpad, Escrow Service, Trading Bot in active development\n🐳BUY HERE: https://t.co/j65N90554E\n\n#CRAOTOKEN  #gems #lowcap #BSCGem #memecoin #BSC #ETH #BTC #SAFEMOON', 'display_text_range': [33, 301], 'entities': {'hashtags': [{'text': 'CRAOTOKEN', 'indices': [233, 243]}, {'text': 'gems', 'indices': [245, 250]}, {'text': 'lowcap', 'indices': [251, 258]}, {'text': 'BSCGem', 'indices': [259, 266]}, {'text': 'memecoin', 'indices': [267, 276]}, {'text': 'BSC', 'indices': [277, 281]}, {'text': 'ETH', 'indices': [282, 286]}, {'text': 'BTC', 'indices': [287, 291]}, {'text': 'SAFEMOON', 'indices': [292, 301]}], 'urls': [{'url': 'https://t.co/j65N90554E', 'expanded_url': 'https://craotoken.com/swap?from=bnb&amp;ref=0xD0956C29c2b5F7012e9Eb4336D67ee0aBde4e906', 'display_url': 'craotoken.com/swap?from=bnb&amp;…', 'indices': [208, 231]}], 'user_mentions': [{'screen_name': 'skulls_humanity', 'name': 'Skulls of Humanity NFT', 'id': 1497133003423768599, 'id_str': '1497133003423768599', 'indices': [0, 16]}, {'screen_name': 'cryptoBILLnfts', 'name': 'Bill ETH', 'id': 2488526546, 'id_str': '2488526546', 'indices': [17, 32]}], 'symbols': []}}</t>
+  </si>
+  <si>
+    <t>$BTC.X 👍</t>
+  </si>
+  <si>
+    <t>05-04-2022 09:35</t>
+  </si>
+  <si>
+    <t>22-02-2022 10:14</t>
+  </si>
+  <si>
+    <t>19-02-2022 14:24</t>
+  </si>
+  <si>
+    <t>21-03-2022 14:17</t>
+  </si>
+  <si>
+    <t>05-04-2022 09:24</t>
+  </si>
+  <si>
+    <t>09-10-2021 14:32</t>
+  </si>
+  <si>
+    <t>14-05-2021 07:37</t>
+  </si>
+  <si>
+    <t>18-03-2022 16:53</t>
+  </si>
+  <si>
+    <t>25-02-2022 08:13</t>
+  </si>
+  <si>
+    <t>31-03-2022 05:38</t>
+  </si>
+  <si>
+    <t>20-03-2010 11:04</t>
   </si>
 </sst>
 </file>
@@ -471,13 +457,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,205 +479,238 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2">
-        <v>96562</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>16</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="E3">
+        <v>53</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4">
-        <v>226</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>37</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6">
-        <v>1905</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>5218</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7">
-        <v>48</v>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>93</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8">
-        <v>42</v>
-      </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>76</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9">
-        <v>42</v>
-      </c>
-      <c r="E9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10">
-        <v>4726</v>
-      </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
         <v>15</v>
       </c>
-      <c r="D11">
-        <v>59</v>
-      </c>
-      <c r="E11" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>